<commit_message>
Maj LAL shade area under ggsurv
</commit_message>
<xml_diff>
--- a/projets/LAL/description_fichier.xlsx
+++ b/projets/LAL/description_fichier.xlsx
@@ -304,7 +304,7 @@
     <t xml:space="preserve">Si non, motif </t>
   </si>
   <si>
-    <t xml:space="preserve">1= pas de prelevemetn; 2=echec; 3=autre motif</t>
+    <t xml:space="preserve">1= pas de prelevement; 2=echec; 3=autre motif</t>
   </si>
   <si>
     <t xml:space="preserve">tECH_IKZF1</t>
@@ -1037,11 +1037,11 @@
   </sheetPr>
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.40625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.37"/>

</xml_diff>